<commit_message>
I MADE IT NEATER
</commit_message>
<xml_diff>
--- a/fyp/matlab/constraint check.xlsx
+++ b/fyp/matlab/constraint check.xlsx
@@ -462,8 +462,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N1044"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16:N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,6 +526,38 @@
         <v>6</v>
       </c>
     </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>0.97040000000000004</v>
+      </c>
+      <c r="F14">
+        <v>2.9600000000000001E-2</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+    </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.97040000000000004</v>
@@ -564,6 +596,36 @@
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2.9600000000000001E-2</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0.91120000000000001</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>8.8800000000000004E-2</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>